<commit_message>
change ui of department and designation + formats
</commit_message>
<xml_diff>
--- a/src/assets/formats/add-new-employee.xlsx
+++ b/src/assets/formats/add-new-employee.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-29475" yWindow="-8700" windowWidth="25605" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="-29475" yWindow="-8700" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -72,15 +72,9 @@
     <t>Aadhaar</t>
   </si>
   <si>
-    <t>Your Organization Name</t>
-  </si>
-  <si>
     <t>Supervisor Code</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Designation Code</t>
   </si>
   <si>
@@ -109,6 +103,12 @@
   </si>
   <si>
     <t>Account Holder Name</t>
+  </si>
+  <si>
+    <t>Contractor</t>
+  </si>
+  <si>
+    <t>Membership Date</t>
   </si>
 </sst>
 </file>
@@ -118,7 +118,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,14 +127,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -178,7 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -193,12 +185,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -470,7 +456,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -478,180 +464,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="9.875" customWidth="1"/>
     <col min="3" max="6" width="22.5" customWidth="1"/>
-    <col min="7" max="9" width="19.125" customWidth="1"/>
-    <col min="10" max="10" width="10.875" style="3"/>
-    <col min="23" max="24" width="14.625" customWidth="1"/>
-    <col min="25" max="25" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.625" style="2" customWidth="1"/>
+    <col min="7" max="11" width="19.125" customWidth="1"/>
+    <col min="12" max="12" width="10.875" style="3"/>
+    <col min="25" max="26" width="14.625" customWidth="1"/>
+    <col min="27" max="27" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:29" s="6" customFormat="1" ht="31.5">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
+      <c r="M1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:27">
-      <c r="A2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
+    <row r="2" spans="1:29">
+      <c r="O2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:27" s="6" customFormat="1" ht="31.5">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA3" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27">
-      <c r="M4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:27">
-      <c r="M5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
+    <row r="3" spans="1:29">
+      <c r="O3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add new feilds to format file
</commit_message>
<xml_diff>
--- a/src/assets/formats/add-new-employee.xlsx
+++ b/src/assets/formats/add-new-employee.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -75,12 +75,6 @@
     <t>Supervisor Code</t>
   </si>
   <si>
-    <t>Designation Code</t>
-  </si>
-  <si>
-    <t>Department Code</t>
-  </si>
-  <si>
     <t>Address Line 1</t>
   </si>
   <si>
@@ -109,6 +103,15 @@
   </si>
   <si>
     <t>Membership Date</t>
+  </si>
+  <si>
+    <t>Designation Name</t>
+  </si>
+  <si>
+    <t>Department Name</t>
+  </si>
+  <si>
+    <t>Branch</t>
   </si>
 </sst>
 </file>
@@ -464,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -479,10 +482,11 @@
     <col min="25" max="26" width="14.625" customWidth="1"/>
     <col min="27" max="27" width="12.875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="21.625" customWidth="1"/>
+    <col min="30" max="30" width="18.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="6" customFormat="1" ht="31.5">
+    <row r="1" spans="1:30" s="6" customFormat="1" ht="31.5">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -493,10 +497,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>3</v>
@@ -505,25 +509,25 @@
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>5</v>
@@ -535,10 +539,10 @@
         <v>7</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>8</v>
@@ -553,13 +557,13 @@
         <v>11</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AA1" s="4" t="s">
         <v>13</v>
@@ -567,17 +571,20 @@
       <c r="AB1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AC1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:30">
       <c r="O2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:30">
       <c r="O3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>

</xml_diff>

<commit_message>
add new fileds to employee edit page and sampe formats
</commit_message>
<xml_diff>
--- a/src/assets/formats/add-new-employee.xlsx
+++ b/src/assets/formats/add-new-employee.xlsx
@@ -22,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Code</t>
   </si>
@@ -112,6 +109,36 @@
   </si>
   <si>
     <t>Contractor Code</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Contractor Name</t>
+  </si>
+  <si>
+    <t>PF NO</t>
+  </si>
+  <si>
+    <t>ESI NO</t>
+  </si>
+  <si>
+    <t>UAN NO</t>
+  </si>
+  <si>
+    <t>Nominee Name</t>
+  </si>
+  <si>
+    <t>Nominee Relation</t>
+  </si>
+  <si>
+    <t>Designation Code</t>
+  </si>
+  <si>
+    <t>Department Code</t>
   </si>
 </sst>
 </file>
@@ -173,21 +200,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -467,122 +508,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AN1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="9.875" customWidth="1"/>
-    <col min="3" max="6" width="22.5" customWidth="1"/>
-    <col min="7" max="11" width="19.125" customWidth="1"/>
-    <col min="12" max="12" width="10.875" style="3"/>
-    <col min="25" max="26" width="14.625" customWidth="1"/>
-    <col min="27" max="27" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.625" customWidth="1"/>
-    <col min="30" max="30" width="18.625" style="2" customWidth="1"/>
+    <col min="3" max="7" width="22.5" customWidth="1"/>
+    <col min="8" max="12" width="19.125" customWidth="1"/>
+    <col min="13" max="13" width="10.875" style="2"/>
+    <col min="28" max="29" width="14.625" customWidth="1"/>
+    <col min="30" max="30" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.625" customWidth="1"/>
+    <col min="33" max="33" width="18.625" style="1" customWidth="1"/>
+    <col min="39" max="39" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="6" customFormat="1" ht="31.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:40" s="4" customFormat="1" ht="31.5">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="AF1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="4" t="s">
+      <c r="AH1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AK1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30">
-      <c r="O2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
+      <c r="AL1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN1" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>